<commit_message>
SqlDatabase Schema in MS SQL , make table
Give Primary Key , Foreign Key
</commit_message>
<xml_diff>
--- a/Database/DatabaseSchemaWebHelperland.xlsx
+++ b/Database/DatabaseSchemaWebHelperland.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Extra\TatvaSoft\SRS\srs\Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BCB6526-96DE-4604-9454-39A26E744B29}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C54C9E-4F8B-4949-80D7-63D652776799}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B57D6876-BB3C-4A12-8958-629A0F235492}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="82">
   <si>
     <t>Admin</t>
   </si>
@@ -250,6 +250,27 @@
   </si>
   <si>
     <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>ServiceProvider</t>
+  </si>
+  <si>
+    <t>ServiceProvider_ID</t>
+  </si>
+  <si>
+    <t>varchar(25)</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>bit</t>
+  </si>
+  <si>
+    <t>Service_Provider_ID</t>
+  </si>
+  <si>
+    <t>Service_Provider</t>
   </si>
 </sst>
 </file>
@@ -300,7 +321,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="15">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -378,6 +399,11 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
       </patternFill>
     </fill>
   </fills>
@@ -558,7 +584,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="14">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -573,8 +599,9 @@
     <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
@@ -604,6 +631,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="13" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="10" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="3" xfId="12" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -616,21 +700,6 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="10" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="4" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="5" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -685,50 +754,17 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="5" xfId="7" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="14" borderId="3" xfId="13" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="4" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="14" borderId="5" xfId="13" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="3" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="4" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="5" xfId="11" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="5" xfId="6" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="3" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="5" xfId="5" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="3" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="4" xfId="14" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="5" xfId="14" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="14">
+  <cellStyles count="15">
     <cellStyle name="20% - Accent1" xfId="4" builtinId="30"/>
     <cellStyle name="20% - Accent6" xfId="12" builtinId="50"/>
     <cellStyle name="40% - Accent2" xfId="7" builtinId="35"/>
@@ -737,6 +773,7 @@
     <cellStyle name="40% - Accent6" xfId="13" builtinId="51"/>
     <cellStyle name="60% - Accent1" xfId="5" builtinId="32"/>
     <cellStyle name="60% - Accent2" xfId="8" builtinId="36"/>
+    <cellStyle name="Accent1" xfId="14" builtinId="29"/>
     <cellStyle name="Accent2" xfId="6" builtinId="33"/>
     <cellStyle name="Accent6" xfId="11" builtinId="49"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -2081,6 +2118,60 @@
         <a:prstGeom prst="line">
           <a:avLst/>
         </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>68580</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>716280</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="26" name="Straight Connector 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBD81EF8-C5EB-49DC-AF2F-D5E464BEE2DC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8999220" y="6461760"/>
+          <a:ext cx="716280" cy="1920240"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:headEnd type="none" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="1">
@@ -2401,8 +2492,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E15EF6A-7421-4C92-A434-4B14D7BE3468}">
   <dimension ref="B2:R53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="P24" sqref="P24"/>
+    <sheetView tabSelected="1" topLeftCell="E28" workbookViewId="0">
+      <selection activeCell="N47" sqref="N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2428,21 +2519,21 @@
   <sheetData>
     <row r="2" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="22"/>
-      <c r="G3" s="29" t="s">
+      <c r="C3" s="35"/>
+      <c r="D3" s="36"/>
+      <c r="G3" s="43" t="s">
         <v>21</v>
       </c>
-      <c r="H3" s="30"/>
-      <c r="I3" s="31"/>
-      <c r="K3" s="17" t="s">
+      <c r="H3" s="44"/>
+      <c r="I3" s="45"/>
+      <c r="K3" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="18"/>
-      <c r="M3" s="19"/>
+      <c r="L3" s="22"/>
+      <c r="M3" s="23"/>
     </row>
     <row r="4" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="4" t="s">
@@ -2574,7 +2665,7 @@
         <v>35</v>
       </c>
       <c r="M9" s="2" t="s">
-        <v>6</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2589,16 +2680,16 @@
       </c>
     </row>
     <row r="11" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G11" s="32" t="s">
+      <c r="G11" s="46" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="33"/>
-      <c r="I11" s="34"/>
-      <c r="P11" s="11" t="s">
+      <c r="H11" s="47"/>
+      <c r="I11" s="48"/>
+      <c r="P11" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="Q11" s="12"/>
-      <c r="R11" s="13"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="32"/>
     </row>
     <row r="12" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G12" s="4" t="s">
@@ -2610,11 +2701,11 @@
       <c r="I12" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="K12" s="47" t="s">
+      <c r="K12" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="15"/>
-      <c r="M12" s="16"/>
+      <c r="L12" s="25"/>
+      <c r="M12" s="26"/>
       <c r="P12" s="9" t="s">
         <v>1</v>
       </c>
@@ -2626,11 +2717,11 @@
       </c>
     </row>
     <row r="13" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="24"/>
-      <c r="D13" s="25"/>
+      <c r="C13" s="38"/>
+      <c r="D13" s="39"/>
       <c r="G13" s="3" t="s">
         <v>4</v>
       </c>
@@ -2717,7 +2808,7 @@
         <v>39</v>
       </c>
       <c r="M15" s="7" t="s">
-        <v>40</v>
+        <v>79</v>
       </c>
       <c r="P15" s="2"/>
       <c r="Q15" s="2" t="s">
@@ -2759,6 +2850,15 @@
       </c>
       <c r="D17" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="P17" s="1"/>
       <c r="Q17" s="10" t="s">
@@ -2790,18 +2890,18 @@
       </c>
     </row>
     <row r="19" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G19" s="35" t="s">
+      <c r="G19" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="H19" s="36"/>
-      <c r="I19" s="37"/>
-      <c r="K19" s="48" t="s">
+      <c r="H19" s="50"/>
+      <c r="I19" s="51"/>
+      <c r="K19" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="L19" s="49"/>
-      <c r="M19" s="50"/>
+      <c r="L19" s="28"/>
+      <c r="M19" s="29"/>
       <c r="P19" s="8"/>
-      <c r="Q19" s="51"/>
+      <c r="Q19" s="11"/>
       <c r="R19" s="8"/>
     </row>
     <row r="20" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2825,11 +2925,11 @@
       </c>
     </row>
     <row r="21" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="26" t="s">
+      <c r="B21" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="C21" s="27"/>
-      <c r="D21" s="28"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="42"/>
       <c r="G21" s="3" t="s">
         <v>4</v>
       </c>
@@ -2930,11 +3030,11 @@
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="H26" s="18"/>
-      <c r="I26" s="19"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="23"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2" t="s">
         <v>49</v>
@@ -2964,11 +3064,11 @@
       </c>
     </row>
     <row r="28" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="41" t="s">
+      <c r="B28" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="43"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="17"/>
       <c r="G28" s="3" t="s">
         <v>4</v>
       </c>
@@ -3005,6 +3105,15 @@
         <v>42</v>
       </c>
       <c r="I29" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M29" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3041,11 +3150,11 @@
       <c r="I31" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="K31" s="14" t="s">
+      <c r="K31" s="33" t="s">
         <v>56</v>
       </c>
-      <c r="L31" s="15"/>
-      <c r="M31" s="16"/>
+      <c r="L31" s="25"/>
+      <c r="M31" s="26"/>
     </row>
     <row r="32" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
@@ -3055,7 +3164,7 @@
         <v>5</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="K32" s="4" t="s">
         <v>1</v>
@@ -3075,13 +3184,13 @@
         <v>36</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G33" s="38" t="s">
+        <v>6</v>
+      </c>
+      <c r="G33" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="H33" s="39"/>
-      <c r="I33" s="40"/>
+      <c r="H33" s="13"/>
+      <c r="I33" s="14"/>
       <c r="K33" s="3" t="s">
         <v>4</v>
       </c>
@@ -3093,9 +3202,15 @@
       </c>
     </row>
     <row r="34" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B34" s="8"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
+      <c r="B34" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>6</v>
+      </c>
       <c r="G34" s="4" t="s">
         <v>1</v>
       </c>
@@ -3143,6 +3258,15 @@
       <c r="I36" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="K36" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="37" spans="2:13" x14ac:dyDescent="0.3">
       <c r="G37" s="2"/>
@@ -3153,7 +3277,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="38" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
         <v>73</v>
@@ -3162,13 +3286,57 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="39" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K39" s="52" t="s">
+        <v>75</v>
+      </c>
+      <c r="L39" s="53"/>
+      <c r="M39" s="54"/>
+    </row>
+    <row r="40" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="M40" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="K41" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="L41" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="M41" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K42" s="7"/>
+      <c r="L42" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="M42" s="7" t="s">
+        <v>77</v>
+      </c>
+    </row>
     <row r="43" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="G43" s="44" t="s">
+      <c r="G43" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="H43" s="45"/>
-      <c r="I43" s="46"/>
+      <c r="H43" s="19"/>
+      <c r="I43" s="20"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="44" spans="2:13" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G44" s="4" t="s">
@@ -3180,6 +3348,13 @@
       <c r="I44" s="6" t="s">
         <v>3</v>
       </c>
+      <c r="K44" s="2"/>
+      <c r="L44" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="M44" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="45" spans="2:13" x14ac:dyDescent="0.3">
       <c r="G45" s="3" t="s">
@@ -3189,6 +3364,15 @@
         <v>64</v>
       </c>
       <c r="I45" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M45" s="2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -3223,19 +3407,24 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="14:14" x14ac:dyDescent="0.3">
+    <row r="49" spans="7:14" x14ac:dyDescent="0.3">
+      <c r="G49" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="53" spans="7:14" x14ac:dyDescent="0.3">
       <c r="N53" t="s">
         <v>74</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="G33:I33"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="G43:I43"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="K12:M12"/>
-    <mergeCell ref="K19:M19"/>
+  <mergeCells count="16">
     <mergeCell ref="P11:R11"/>
     <mergeCell ref="K31:M31"/>
     <mergeCell ref="G26:I26"/>
@@ -3245,6 +3434,13 @@
     <mergeCell ref="G3:I3"/>
     <mergeCell ref="G11:I11"/>
     <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G33:I33"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="G43:I43"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="K12:M12"/>
+    <mergeCell ref="K19:M19"/>
+    <mergeCell ref="K39:M39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>